<commit_message>
charts for 4 osds vary num objs experiments.
</commit_message>
<xml_diff>
--- a/src/progly/cloudlab_vary_nobjs_experiment/4osds-g1/google-spreadsheet-vary-nobjs.xlsx
+++ b/src/progly/cloudlab_vary_nobjs_experiment/4osds-g1/google-spreadsheet-vary-nobjs.xlsx
@@ -4,9 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="data" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="chart-store-index-objs" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="chart-query" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="chart-hotcache" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="chart-vary-nobjs-store-index" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="chart-vary-nobjs-query" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="chart-vary-nobjs-hotcache" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -319,11 +319,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1395143946"/>
-        <c:axId val="72882739"/>
+        <c:axId val="115632823"/>
+        <c:axId val="158050653"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1395143946"/>
+        <c:axId val="115632823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,10 +355,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72882739"/>
+        <c:crossAx val="158050653"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72882739"/>
+        <c:axId val="158050653"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -415,7 +415,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1395143946"/>
+        <c:crossAx val="115632823"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -603,11 +603,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1403490840"/>
-        <c:axId val="1492825256"/>
+        <c:axId val="1404998407"/>
+        <c:axId val="887554864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1403490840"/>
+        <c:axId val="1404998407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,10 +639,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1492825256"/>
+        <c:crossAx val="887554864"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1492825256"/>
+        <c:axId val="887554864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,18 +699,18 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1403490840"/>
+        <c:crossAx val="1404998407"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0">
-            <a:defRPr sz="1400"/>
+            <a:defRPr sz="1200"/>
           </a:pPr>
         </a:p>
       </c:txPr>
@@ -863,11 +863,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1512937205"/>
-        <c:axId val="2119626185"/>
+        <c:axId val="1086002843"/>
+        <c:axId val="2003108444"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1512937205"/>
+        <c:axId val="1086002843"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,10 +882,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119626185"/>
+        <c:crossAx val="2003108444"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119626185"/>
+        <c:axId val="2003108444"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1512937205"/>
+        <c:crossAx val="1086002843"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1000,7 +1000,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1025,7 +1025,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1050,7 +1050,7 @@
     <xdr:ext cx="8610600" cy="6276975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>

</xml_diff>

<commit_message>
only changed titles+legend from 'scan query' to 'range query'.
</commit_message>
<xml_diff>
--- a/src/progly/cloudlab_vary_nobjs_experiment/4osds-g1/google-spreadsheet-vary-nobjs.xlsx
+++ b/src/progly/cloudlab_vary_nobjs_experiment/4osds-g1/google-spreadsheet-vary-nobjs.xlsx
@@ -94,13 +94,13 @@
     <t>query data</t>
   </si>
   <si>
-    <t>client-scan-query</t>
+    <t>client-range-query</t>
   </si>
   <si>
     <t>client-point-query</t>
   </si>
   <si>
-    <t>server-scan-query</t>
+    <t>server-range-query</t>
   </si>
   <si>
     <t>server-point-query</t>
@@ -260,7 +260,7 @@
               <a:defRPr sz="1400"/>
             </a:pPr>
             <a:r>
-              <a:t>4OSDs: Median time for varying number of objects (1B rows/140GB dataset)</a:t>
+              <a:t>4OSDs: Median time for varying number of objects (1B rows/140GB TPC-H dataset)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -319,11 +319,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="115632823"/>
-        <c:axId val="158050653"/>
+        <c:axId val="193158453"/>
+        <c:axId val="957114153"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115632823"/>
+        <c:axId val="193158453"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,10 +355,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158050653"/>
+        <c:crossAx val="957114153"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158050653"/>
+        <c:axId val="957114153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -415,7 +415,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115632823"/>
+        <c:crossAx val="193158453"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -448,7 +448,7 @@
               <a:defRPr sz="1400"/>
             </a:pPr>
             <a:r>
-              <a:t>4OSDs: Median time for scan (s=10%) and point query (unique record), client-side vs. server-side processing (pushdown)</a:t>
+              <a:t>4OSDs: Median time for range (s=10%) and point query (unique record), client-side vs. server-side processing (storage pushdown)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -603,11 +603,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1404998407"/>
-        <c:axId val="887554864"/>
+        <c:axId val="2089163268"/>
+        <c:axId val="56089729"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1404998407"/>
+        <c:axId val="2089163268"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,10 +639,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="887554864"/>
+        <c:crossAx val="56089729"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="887554864"/>
+        <c:axId val="56089729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +699,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1404998407"/>
+        <c:crossAx val="2089163268"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -732,7 +732,7 @@
               <a:defRPr sz="1600"/>
             </a:pPr>
             <a:r>
-              <a:t>4OSDs: Median time for scan (s=10%) and point query (unique record), client-side vs. server-side processing (pushdown)</a:t>
+              <a:t>4OSDs: Median time for range (s=10%) and point query (unique record), client-side vs. server-side processing (storage pushdown)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -863,11 +863,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1086002843"/>
-        <c:axId val="2003108444"/>
+        <c:axId val="1617939550"/>
+        <c:axId val="155549848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1086002843"/>
+        <c:axId val="1617939550"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,10 +882,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2003108444"/>
+        <c:crossAx val="155549848"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2003108444"/>
+        <c:axId val="155549848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1086002843"/>
+        <c:crossAx val="1617939550"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>